<commit_message>
v.6 : Pagination enhancement
</commit_message>
<xml_diff>
--- a/Data/Group.xlsx
+++ b/Data/Group.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -194,11 +193,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -393,8 +392,8 @@
   </sheetPr>
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,28 +418,116 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -450,138 +537,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A22"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>